<commit_message>
remove plate 1 from Fig 4 and Suppl table 1
</commit_message>
<xml_diff>
--- a/SVGs/SupplTable_1.xlsx
+++ b/SVGs/SupplTable_1.xlsx
@@ -747,8 +747,8 @@
   </sheetPr>
   <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -839,7 +839,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="22" t="n">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F5" s="23" t="n">
         <v>0</v>
@@ -849,7 +849,7 @@
       </c>
       <c r="H5" s="25" t="n">
         <f aca="false">SUM(E5:G5)</f>
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="11" t="s">
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="27" t="n">
-        <v>0.949348827403542</v>
+        <v>0.929953380101468</v>
       </c>
       <c r="M5" s="28" t="s">
         <v>10</v>
@@ -872,14 +872,14 @@
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
     </row>
-    <row r="6" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="32" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F6" s="8" t="n">
         <v>2</v>
@@ -889,68 +889,68 @@
       </c>
       <c r="H6" s="34" t="n">
         <f aca="false">SUM(E6:G6)</f>
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="J6" s="35" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="36" t="n">
-        <v>0.895833333333333</v>
+        <v>0.852941176470588</v>
       </c>
       <c r="L6" s="30" t="n">
-        <v>0.778325783056137</v>
+        <v>0.698719435045478</v>
       </c>
       <c r="M6" s="37" t="s">
         <v>10</v>
       </c>
       <c r="N6" s="38" t="n">
-        <v>0.954678280958187</v>
+        <v>0.935505585552175</v>
       </c>
       <c r="P6" s="30"/>
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
       <c r="S6" s="30"/>
     </row>
-    <row r="7" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="31" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="8" t="n">
         <v>2</v>
       </c>
       <c r="G7" s="33" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H7" s="34" t="n">
         <f aca="false">SUM(E7:G7)</f>
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J7" s="35" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="36" t="n">
-        <v>0.228571428571429</v>
+        <v>0.304347826086957</v>
       </c>
       <c r="L7" s="30" t="n">
-        <v>0.120658798341917</v>
+        <v>0.15604024453214</v>
       </c>
       <c r="M7" s="37" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="38" t="n">
-        <v>0.390173168919902</v>
+        <v>0.508657562687592</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
       <c r="D8" s="39" t="s">
@@ -990,7 +990,7 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="19"/>
       <c r="C9" s="48" t="s">
         <v>4</v>
@@ -1005,11 +1005,11 @@
         <v>13</v>
       </c>
       <c r="G9" s="52" t="n">
-        <v>696</v>
+        <v>648</v>
       </c>
       <c r="H9" s="53" t="n">
         <f aca="false">SUM(E9:G9)</f>
-        <v>711</v>
+        <v>663</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="54"/>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="E10" s="41" t="n">
         <f aca="false">SUM(E5:E9)</f>
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="F10" s="41" t="n">
         <f aca="false">SUM(F5:F9)</f>
@@ -1037,11 +1037,11 @@
       </c>
       <c r="G10" s="42" t="n">
         <f aca="false">SUM(G5:G9)</f>
-        <v>744</v>
+        <v>685</v>
       </c>
       <c r="H10" s="56" t="n">
         <f aca="false">SUM(E10:G10)</f>
-        <v>887</v>
+        <v>792</v>
       </c>
       <c r="K10" s="57"/>
       <c r="L10" s="58"/>
@@ -1058,19 +1058,19 @@
       <c r="M11" s="61"/>
       <c r="N11" s="61"/>
     </row>
-    <row r="12" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="62"/>
       <c r="K12" s="63" t="n">
-        <v>0.997134670487106</v>
+        <v>0.996923076923077</v>
       </c>
       <c r="L12" s="64" t="n">
-        <v>0.989613436182212</v>
+        <v>0.988851303740987</v>
       </c>
       <c r="M12" s="65" t="s">
         <v>10</v>
       </c>
       <c r="N12" s="66" t="n">
-        <v>0.999213871292798</v>
+        <v>0.999155790769604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lowercase interval in Sup tab 1
</commit_message>
<xml_diff>
--- a/SVGs/SupplTable_1.xlsx
+++ b/SVGs/SupplTable_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t xml:space="preserve">RT-LAMP
 Result </t>
@@ -32,6 +32,9 @@
     <t xml:space="preserve">pos</t>
   </si>
   <si>
+    <t xml:space="preserve">inc.</t>
+  </si>
+  <si>
     <t xml:space="preserve">neg</t>
   </si>
   <si>
@@ -41,7 +44,7 @@
     <t xml:space="preserve">Sensitivity</t>
   </si>
   <si>
-    <t xml:space="preserve">95% conf. Int.</t>
+    <t xml:space="preserve">95% conf. int.</t>
   </si>
   <si>
     <t xml:space="preserve">RT-qPCR
@@ -138,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -162,6 +165,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="double"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right/>
       <top style="thin"/>
       <bottom/>
@@ -232,6 +242,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right/>
+      <top style="double"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="double"/>
       <top style="double"/>
       <bottom/>
@@ -240,13 +257,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
@@ -295,14 +305,14 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="double"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
@@ -389,7 +399,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -406,6 +416,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -442,43 +456,51 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,15 +508,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,27 +524,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -530,27 +552,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,43 +588,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -614,11 +640,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,19 +652,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -719,316 +745,341 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AMJ12"/>
+  <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="209" zoomScaleNormal="209" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="3.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="5.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="4.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="19" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="3.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="20" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="J3" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="K3" s="7"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="7"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-    </row>
-    <row r="4" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="10" t="s">
+      <c r="M3" s="9"/>
+      <c r="N3" s="8"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" s="10" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="H4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="22" t="n">
+        <v>51</v>
+      </c>
+      <c r="F5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="25" t="n">
+        <f aca="false">SUM(E5:G5)</f>
+        <v>51</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27" t="n">
+        <v>0.929953380101468</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="32" t="n">
+        <v>29</v>
+      </c>
+      <c r="F6" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="K4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17" t="s">
+      <c r="H6" s="34" t="n">
+        <f aca="false">SUM(E6:G6)</f>
+        <v>36</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="36" t="n">
+        <v>0.852941176470588</v>
+      </c>
+      <c r="L6" s="30" t="n">
+        <v>0.698719435045478</v>
+      </c>
+      <c r="M6" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="38" t="n">
+        <v>0.935505585552175</v>
+      </c>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="F7" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="20" t="n">
-        <v>51</v>
-      </c>
-      <c r="F5" s="21" t="n">
+      <c r="G7" s="33" t="n">
+        <v>16</v>
+      </c>
+      <c r="H7" s="34" t="n">
+        <f aca="false">SUM(E7:G7)</f>
+        <v>25</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="36" t="n">
+        <v>0.304347826086957</v>
+      </c>
+      <c r="L7" s="30" t="n">
+        <v>0.15604024453214</v>
+      </c>
+      <c r="M7" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="38" t="n">
+        <v>0.508657562687592</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="22" t="n">
-        <f aca="false">SUM(E5:F5)</f>
-        <v>51</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="24" t="n">
-        <v>0.929953380101468</v>
-      </c>
-      <c r="L5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="28" t="s">
+      <c r="G8" s="42" t="n">
+        <v>16</v>
+      </c>
+      <c r="H8" s="34" t="n">
+        <f aca="false">SUM(E8:G8)</f>
+        <v>17</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="44" t="n">
+        <v>0.0588235294117647</v>
+      </c>
+      <c r="L8" s="45" t="n">
+        <v>0.0104604009849976</v>
+      </c>
+      <c r="M8" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="29" t="n">
-        <v>29</v>
-      </c>
-      <c r="F6" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="G6" s="31" t="n">
-        <f aca="false">SUM(E6:F6)</f>
-        <v>36</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="33" t="n">
-        <v>0.805555555555556</v>
-      </c>
-      <c r="K6" s="27" t="n">
-        <v>0.649719570048226</v>
-      </c>
-      <c r="L6" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="35" t="n">
-        <v>0.902469045810713</v>
-      </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="29" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" s="30" t="n">
-        <v>18</v>
-      </c>
-      <c r="G7" s="31" t="n">
-        <f aca="false">SUM(E7:F7)</f>
-        <v>25</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="33" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="K7" s="27" t="n">
-        <v>0.142838538509566</v>
-      </c>
-      <c r="L7" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="35" t="n">
-        <v>0.475766051903616</v>
-      </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="38" t="n">
-        <v>16</v>
-      </c>
-      <c r="G8" s="31" t="n">
-        <f aca="false">SUM(E8:F8)</f>
-        <v>17</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="40" t="n">
-        <v>0.0588235294117647</v>
-      </c>
-      <c r="K8" s="41" t="n">
-        <v>0.0104604009849976</v>
-      </c>
-      <c r="L8" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="43" t="n">
+      <c r="N8" s="47" t="n">
         <v>0.269820306375754</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="17"/>
-      <c r="C9" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="46" t="n">
+      <c r="B9" s="19"/>
+      <c r="C9" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="47" t="n">
-        <v>661</v>
-      </c>
-      <c r="G9" s="48" t="n">
-        <f aca="false">SUM(E9:F9)</f>
+      <c r="F9" s="51" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" s="52" t="n">
+        <v>648</v>
+      </c>
+      <c r="H9" s="53" t="n">
+        <f aca="false">SUM(E9:G9)</f>
         <v>663</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="51" t="n">
+      <c r="I9" s="8"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="41" t="n">
         <f aca="false">SUM(E5:E9)</f>
         <v>90</v>
       </c>
-      <c r="F10" s="38" t="n">
+      <c r="F10" s="41" t="n">
         <f aca="false">SUM(F5:F9)</f>
-        <v>702</v>
-      </c>
-      <c r="G10" s="52" t="n">
-        <f aca="false">SUM(E10:F10)</f>
+        <v>17</v>
+      </c>
+      <c r="G10" s="42" t="n">
+        <f aca="false">SUM(G5:G9)</f>
+        <v>685</v>
+      </c>
+      <c r="H10" s="56" t="n">
+        <f aca="false">SUM(E10:G10)</f>
         <v>792</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="54"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="57" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="58"/>
+    </row>
+    <row r="11" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K11" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="58"/>
-      <c r="J12" s="59" t="n">
-        <v>0.996983408748114</v>
-      </c>
-      <c r="K12" s="60" t="n">
-        <v>0.989068543164947</v>
-      </c>
-      <c r="L12" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="62" t="n">
-        <v>0.999172351702985</v>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63" t="n">
+        <v>0.996923076923077</v>
+      </c>
+      <c r="L12" s="64" t="n">
+        <v>0.988851303740987</v>
+      </c>
+      <c r="M12" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="66" t="n">
+        <v>0.999155790769604</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="L4:N4"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="C5:C8"/>
-    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="L11:N11"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
exclude wells with wellRemark (ctrls, beads)
</commit_message>
<xml_diff>
--- a/SVGs/SupplTable_1.xlsx
+++ b/SVGs/SupplTable_1.xlsx
@@ -721,8 +721,8 @@
   </sheetPr>
   <dimension ref="B1:AMJ12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -837,116 +837,116 @@
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
     </row>
-    <row r="6" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="28" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="29" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="30" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6" s="31" t="n">
         <f aca="false">SUM(E6:F6)</f>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I6" s="32" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="33" t="n">
-        <v>0.8055556</v>
+        <v>0.933333333333333</v>
       </c>
       <c r="K6" s="27" t="n">
-        <v>0.6497196</v>
+        <v>0.786765416373831</v>
       </c>
       <c r="L6" s="34" t="s">
         <v>9</v>
       </c>
       <c r="M6" s="35" t="n">
-        <v>0.902469</v>
+        <v>0.98152297620873</v>
       </c>
       <c r="O6" s="27"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
     </row>
-    <row r="7" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="29" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F7" s="30" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" s="31" t="n">
         <f aca="false">SUM(E7:F7)</f>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I7" s="32" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="33" t="n">
-        <v>0.28</v>
+        <v>0.2</v>
       </c>
       <c r="K7" s="27" t="n">
-        <v>0.1428385</v>
+        <v>0.0806576625797981</v>
       </c>
       <c r="L7" s="34" t="s">
         <v>9</v>
       </c>
       <c r="M7" s="35" t="n">
-        <v>0.4757661</v>
+        <v>0.416017432251894</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
       <c r="D8" s="36" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="38" t="n">
         <v>16</v>
       </c>
       <c r="G8" s="31" t="n">
         <f aca="false">SUM(E8:F8)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="39" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="40" t="n">
-        <v>0.05882353</v>
+        <v>0</v>
       </c>
       <c r="K8" s="41" t="n">
-        <v>0.0104604</v>
+        <v>0</v>
       </c>
       <c r="L8" s="42" t="s">
         <v>9</v>
       </c>
       <c r="M8" s="43" t="n">
-        <v>0.2698203</v>
+        <v>0.193607680534436</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="17"/>
       <c r="C9" s="44" t="s">
         <v>3</v>
@@ -958,11 +958,11 @@
         <v>2</v>
       </c>
       <c r="F9" s="47" t="n">
-        <v>661</v>
+        <v>649</v>
       </c>
       <c r="G9" s="48" t="n">
         <f aca="false">SUM(E9:F9)</f>
-        <v>663</v>
+        <v>651</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="49"/>
@@ -982,15 +982,15 @@
       </c>
       <c r="E10" s="51" t="n">
         <f aca="false">SUM(E5:E9)</f>
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F10" s="38" t="n">
         <f aca="false">SUM(F5:F9)</f>
-        <v>702</v>
+        <v>683</v>
       </c>
       <c r="G10" s="52" t="n">
         <f aca="false">SUM(E10:F10)</f>
-        <v>792</v>
+        <v>768</v>
       </c>
       <c r="J10" s="53"/>
       <c r="K10" s="54"/>
@@ -1007,10 +1007,10 @@
       <c r="L11" s="57"/>
       <c r="M11" s="57"/>
     </row>
-    <row r="12" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I12" s="58"/>
       <c r="J12" s="59" t="n">
-        <v>0.9969834</v>
+        <v>0.996927803379416</v>
       </c>
       <c r="K12" s="60" t="n">
         <v>0.9890685</v>

</xml_diff>